<commit_message>
all good fix pengujian
</commit_message>
<xml_diff>
--- a/Hasil_Pengujian_Map_128.xlsx
+++ b/Hasil_Pengujian_Map_128.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.000798</v>
+        <v>0.0007784000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00433</v>
+        <v>0.004484399999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03118</v>
+        <v>0.0302263</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2027</v>
+        <v>0.2061969</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.000463</v>
+        <v>0.0004272</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001639</v>
+        <v>0.0015999</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006339</v>
+        <v>0.006348000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>0.026478</v>
+        <v>0.0268846</v>
       </c>
     </row>
     <row r="4">
@@ -523,16 +523,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0009</v>
+        <v>0.0009392</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004416</v>
+        <v>0.004326200000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>0.027277</v>
+        <v>0.0267379</v>
       </c>
       <c r="F4" t="n">
-        <v>0.194389</v>
+        <v>0.1837008</v>
       </c>
     </row>
     <row r="5">
@@ -545,16 +545,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.000789</v>
+        <v>0.0008022000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>0.004292</v>
+        <v>0.0041335</v>
       </c>
       <c r="E5" t="n">
-        <v>0.027439</v>
+        <v>0.0270095</v>
       </c>
       <c r="F5" t="n">
-        <v>0.18601</v>
+        <v>0.1825045</v>
       </c>
     </row>
     <row r="6">
@@ -567,16 +567,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.0005820000000000001</v>
+        <v>0.000547</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001967</v>
+        <v>0.0019546</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00758</v>
+        <v>0.007536099999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>0.028951</v>
+        <v>0.0289774</v>
       </c>
     </row>
     <row r="7">
@@ -589,16 +589,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.000846</v>
+        <v>0.000826</v>
       </c>
       <c r="D7" t="n">
-        <v>0.004547</v>
+        <v>0.004412399999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>0.029762</v>
+        <v>0.0297573</v>
       </c>
       <c r="F7" t="n">
-        <v>0.201216</v>
+        <v>0.206724</v>
       </c>
     </row>
     <row r="8">
@@ -611,16 +611,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0008229999999999999</v>
+        <v>0.0008253000000000002</v>
       </c>
       <c r="D8" t="n">
-        <v>0.004704</v>
+        <v>0.0044815</v>
       </c>
       <c r="E8" t="n">
-        <v>0.029886</v>
+        <v>0.0300391</v>
       </c>
       <c r="F8" t="n">
-        <v>0.198207</v>
+        <v>0.2013994</v>
       </c>
     </row>
     <row r="9">
@@ -633,16 +633,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.000593</v>
+        <v>0.0005342</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00268</v>
+        <v>0.0024626</v>
       </c>
       <c r="E9" t="n">
-        <v>0.010957</v>
+        <v>0.0108098</v>
       </c>
       <c r="F9" t="n">
-        <v>0.056574</v>
+        <v>0.0546881</v>
       </c>
     </row>
     <row r="10">
@@ -655,16 +655,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.000354</v>
+        <v>0.000342</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001648</v>
+        <v>0.0016111</v>
       </c>
       <c r="E10" t="n">
-        <v>0.007148</v>
+        <v>0.007117800000000001</v>
       </c>
       <c r="F10" t="n">
-        <v>0.031042</v>
+        <v>0.031061</v>
       </c>
     </row>
     <row r="11">
@@ -677,16 +677,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.000465</v>
+        <v>0.0004395000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00185</v>
+        <v>0.0017218</v>
       </c>
       <c r="E11" t="n">
-        <v>0.006699</v>
+        <v>0.0067505</v>
       </c>
       <c r="F11" t="n">
-        <v>0.027686</v>
+        <v>0.0278521</v>
       </c>
     </row>
     <row r="12">
@@ -699,16 +699,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.000455</v>
+        <v>0.0004638</v>
       </c>
       <c r="D12" t="n">
-        <v>0.001805</v>
+        <v>0.0018252</v>
       </c>
       <c r="E12" t="n">
-        <v>0.006948</v>
+        <v>0.0066718</v>
       </c>
       <c r="F12" t="n">
-        <v>0.029499</v>
+        <v>0.0282039</v>
       </c>
     </row>
     <row r="13">
@@ -721,16 +721,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0009389999999999999</v>
+        <v>0.0009023000000000002</v>
       </c>
       <c r="D13" t="n">
-        <v>0.004583</v>
+        <v>0.0044641</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02738</v>
+        <v>0.0272446</v>
       </c>
       <c r="F13" t="n">
-        <v>0.187777</v>
+        <v>0.1834948</v>
       </c>
     </row>
     <row r="14">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.000992</v>
+        <v>0.0009879999999999997</v>
       </c>
       <c r="D14" t="n">
-        <v>0.004864</v>
+        <v>0.0046515</v>
       </c>
       <c r="E14" t="n">
-        <v>0.031048</v>
+        <v>0.0311564</v>
       </c>
       <c r="F14" t="n">
-        <v>0.205793</v>
+        <v>0.2019104</v>
       </c>
     </row>
     <row r="15">
@@ -765,16 +765,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.001061</v>
+        <v>0.0009778999999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>0.006346</v>
+        <v>0.0057486</v>
       </c>
       <c r="E15" t="n">
-        <v>0.034942</v>
+        <v>0.0343722</v>
       </c>
       <c r="F15" t="n">
-        <v>0.23567</v>
+        <v>0.2309405</v>
       </c>
     </row>
     <row r="16">
@@ -787,16 +787,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.00083</v>
+        <v>0.0008128</v>
       </c>
       <c r="D16" t="n">
-        <v>0.004419</v>
+        <v>0.004266299999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>0.027643</v>
+        <v>0.0272314</v>
       </c>
       <c r="F16" t="n">
-        <v>0.188419</v>
+        <v>0.1838681</v>
       </c>
     </row>
     <row r="17">
@@ -809,16 +809,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.00081</v>
+        <v>0.000791</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00478</v>
+        <v>0.0044435</v>
       </c>
       <c r="E17" t="n">
-        <v>0.027522</v>
+        <v>0.0269114</v>
       </c>
       <c r="F17" t="n">
-        <v>0.174215</v>
+        <v>0.1708793</v>
       </c>
     </row>
     <row r="18">
@@ -831,16 +831,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.000462</v>
+        <v>0.0004343</v>
       </c>
       <c r="D18" t="n">
-        <v>0.001429</v>
+        <v>0.0014483</v>
       </c>
       <c r="E18" t="n">
-        <v>0.004733</v>
+        <v>0.004667500000000001</v>
       </c>
       <c r="F18" t="n">
-        <v>0.016592</v>
+        <v>0.0167271</v>
       </c>
     </row>
     <row r="19">
@@ -853,16 +853,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.000502</v>
+        <v>0.0004690999999999999</v>
       </c>
       <c r="D19" t="n">
-        <v>0.001544</v>
+        <v>0.001471</v>
       </c>
       <c r="E19" t="n">
-        <v>0.004502</v>
+        <v>0.0044715</v>
       </c>
       <c r="F19" t="n">
-        <v>0.015106</v>
+        <v>0.0153374</v>
       </c>
     </row>
     <row r="20">
@@ -875,16 +875,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.000581</v>
+        <v>0.0005941</v>
       </c>
       <c r="D20" t="n">
-        <v>0.001786</v>
+        <v>0.0017534</v>
       </c>
       <c r="E20" t="n">
-        <v>0.006503</v>
+        <v>0.006178399999999999</v>
       </c>
       <c r="F20" t="n">
-        <v>0.022944</v>
+        <v>0.0233091</v>
       </c>
     </row>
     <row r="21">
@@ -897,16 +897,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.0005730000000000001</v>
+        <v>0.0005989000000000001</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002024</v>
+        <v>0.0019967</v>
       </c>
       <c r="E21" t="n">
-        <v>0.007841000000000001</v>
+        <v>0.007582299999999998</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02971</v>
+        <v>0.0290922</v>
       </c>
     </row>
     <row r="22">
@@ -919,16 +919,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.00059</v>
+        <v>0.0005779</v>
       </c>
       <c r="D22" t="n">
-        <v>0.002161</v>
+        <v>0.0022348</v>
       </c>
       <c r="E22" t="n">
-        <v>0.008148000000000001</v>
+        <v>0.008144799999999999</v>
       </c>
       <c r="F22" t="n">
-        <v>0.032547</v>
+        <v>0.0315793</v>
       </c>
     </row>
     <row r="23">
@@ -941,16 +941,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.000876</v>
+        <v>0.0008611000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>0.004678</v>
+        <v>0.0045859</v>
       </c>
       <c r="E23" t="n">
-        <v>0.030131</v>
+        <v>0.0302272</v>
       </c>
       <c r="F23" t="n">
-        <v>0.200308</v>
+        <v>0.2029765</v>
       </c>
     </row>
     <row r="24">
@@ -963,16 +963,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.000593</v>
+        <v>0.0005696</v>
       </c>
       <c r="D24" t="n">
-        <v>0.002666</v>
+        <v>0.0025734</v>
       </c>
       <c r="E24" t="n">
-        <v>0.011354</v>
+        <v>0.0112496</v>
       </c>
       <c r="F24" t="n">
-        <v>0.057007</v>
+        <v>0.0555345</v>
       </c>
     </row>
     <row r="25">
@@ -985,16 +985,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.000601</v>
+        <v>0.0005897</v>
       </c>
       <c r="D25" t="n">
-        <v>0.002514</v>
+        <v>0.002391</v>
       </c>
       <c r="E25" t="n">
-        <v>0.012018</v>
+        <v>0.011818</v>
       </c>
       <c r="F25" t="n">
-        <v>0.056834</v>
+        <v>0.0550076</v>
       </c>
     </row>
     <row r="26">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.000562</v>
+        <v>0.0005288</v>
       </c>
       <c r="D26" t="n">
-        <v>0.002816</v>
+        <v>0.0026704</v>
       </c>
       <c r="E26" t="n">
-        <v>0.012364</v>
+        <v>0.0117298</v>
       </c>
       <c r="F26" t="n">
-        <v>0.061122</v>
+        <v>0.05915459999999999</v>
       </c>
     </row>
     <row r="27">
@@ -1029,16 +1029,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.000398</v>
+        <v>0.0003914</v>
       </c>
       <c r="D27" t="n">
-        <v>0.00178</v>
+        <v>0.0017136</v>
       </c>
       <c r="E27" t="n">
-        <v>0.007427</v>
+        <v>0.007401799999999998</v>
       </c>
       <c r="F27" t="n">
-        <v>0.031872</v>
+        <v>0.03222399999999999</v>
       </c>
     </row>
     <row r="28">
@@ -1051,16 +1051,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.000428</v>
+        <v>0.000406</v>
       </c>
       <c r="D28" t="n">
-        <v>0.001726</v>
+        <v>0.0017109</v>
       </c>
       <c r="E28" t="n">
-        <v>0.007138</v>
+        <v>0.0072299</v>
       </c>
       <c r="F28" t="n">
-        <v>0.031692</v>
+        <v>0.0320002</v>
       </c>
     </row>
     <row r="29">
@@ -1073,16 +1073,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.0005240000000000001</v>
+        <v>0.0004809</v>
       </c>
       <c r="D29" t="n">
-        <v>0.001909</v>
+        <v>0.0019201</v>
       </c>
       <c r="E29" t="n">
-        <v>0.007116</v>
+        <v>0.007023699999999999</v>
       </c>
       <c r="F29" t="n">
-        <v>0.029767</v>
+        <v>0.0293574</v>
       </c>
     </row>
     <row r="30">
@@ -1095,16 +1095,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.001039</v>
+        <v>0.0010377</v>
       </c>
       <c r="D30" t="n">
-        <v>0.004879</v>
+        <v>0.0048422</v>
       </c>
       <c r="E30" t="n">
-        <v>0.031437</v>
+        <v>0.0316909</v>
       </c>
       <c r="F30" t="n">
-        <v>0.206039</v>
+        <v>0.2019355</v>
       </c>
     </row>
     <row r="31">
@@ -1117,16 +1117,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.001201</v>
+        <v>0.0010183</v>
       </c>
       <c r="D31" t="n">
-        <v>0.005883</v>
+        <v>0.0058763</v>
       </c>
       <c r="E31" t="n">
-        <v>0.035825</v>
+        <v>0.0348778</v>
       </c>
       <c r="F31" t="n">
-        <v>0.237234</v>
+        <v>0.2313516</v>
       </c>
     </row>
     <row r="32">
@@ -1139,16 +1139,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.001041</v>
+        <v>0.0010351</v>
       </c>
       <c r="D32" t="n">
-        <v>0.006039</v>
+        <v>0.0059809</v>
       </c>
       <c r="E32" t="n">
-        <v>0.036033</v>
+        <v>0.0344764</v>
       </c>
       <c r="F32" t="n">
-        <v>0.228404</v>
+        <v>0.22421</v>
       </c>
     </row>
     <row r="33">
@@ -1161,16 +1161,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.00086</v>
+        <v>0.0008521000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>0.004597</v>
+        <v>0.0045752</v>
       </c>
       <c r="E33" t="n">
-        <v>0.026879</v>
+        <v>0.0268791</v>
       </c>
       <c r="F33" t="n">
-        <v>0.174782</v>
+        <v>0.1722595</v>
       </c>
     </row>
     <row r="34">
@@ -1183,16 +1183,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.000451</v>
+        <v>0.0004306</v>
       </c>
       <c r="D34" t="n">
-        <v>0.001283</v>
+        <v>0.0012812</v>
       </c>
       <c r="E34" t="n">
-        <v>0.004003</v>
+        <v>0.004025900000000001</v>
       </c>
       <c r="F34" t="n">
-        <v>0.013824</v>
+        <v>0.0139221</v>
       </c>
     </row>
     <row r="35">
@@ -1205,16 +1205,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.000288</v>
+        <v>0.0002615</v>
       </c>
       <c r="D35" t="n">
-        <v>0.000889</v>
+        <v>0.0008653000000000001</v>
       </c>
       <c r="E35" t="n">
-        <v>0.003007</v>
+        <v>0.0028675</v>
       </c>
       <c r="F35" t="n">
-        <v>0.010743</v>
+        <v>0.0108575</v>
       </c>
     </row>
     <row r="36">
@@ -1227,16 +1227,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.000481</v>
+        <v>0.0004661999999999999</v>
       </c>
       <c r="D36" t="n">
-        <v>0.001482</v>
+        <v>0.0015102</v>
       </c>
       <c r="E36" t="n">
-        <v>0.004795</v>
+        <v>0.0047268</v>
       </c>
       <c r="F36" t="n">
-        <v>0.016961</v>
+        <v>0.016908</v>
       </c>
     </row>
     <row r="37">
@@ -1249,16 +1249,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.000407</v>
+        <v>0.0003911</v>
       </c>
       <c r="D37" t="n">
-        <v>0.001178</v>
+        <v>0.0011544</v>
       </c>
       <c r="E37" t="n">
-        <v>0.004045</v>
+        <v>0.0040903</v>
       </c>
       <c r="F37" t="n">
-        <v>0.018556</v>
+        <v>0.0184192</v>
       </c>
     </row>
     <row r="38">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.00052</v>
+        <v>0.0004972000000000001</v>
       </c>
       <c r="D38" t="n">
-        <v>0.001556</v>
+        <v>0.0015433</v>
       </c>
       <c r="E38" t="n">
-        <v>0.004711</v>
+        <v>0.004513000000000001</v>
       </c>
       <c r="F38" t="n">
-        <v>0.015605</v>
+        <v>0.0153167</v>
       </c>
     </row>
     <row r="39">
@@ -1293,16 +1293,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.000499</v>
+        <v>0.0004627</v>
       </c>
       <c r="D39" t="n">
-        <v>0.001487</v>
+        <v>0.0022169</v>
       </c>
       <c r="E39" t="n">
-        <v>0.003867</v>
+        <v>0.0038426</v>
       </c>
       <c r="F39" t="n">
-        <v>0.012889</v>
+        <v>0.0130456</v>
       </c>
     </row>
     <row r="40">
@@ -1315,16 +1315,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.0005240000000000001</v>
+        <v>0.0005283</v>
       </c>
       <c r="D40" t="n">
-        <v>0.001589</v>
+        <v>0.0016104</v>
       </c>
       <c r="E40" t="n">
-        <v>0.004675</v>
+        <v>0.0045105</v>
       </c>
       <c r="F40" t="n">
-        <v>0.017927</v>
+        <v>0.0167207</v>
       </c>
     </row>
     <row r="41">
@@ -1337,16 +1337,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.000594</v>
+        <v>0.0010529</v>
       </c>
       <c r="D41" t="n">
-        <v>0.001798</v>
+        <v>0.0017938</v>
       </c>
       <c r="E41" t="n">
-        <v>0.006514</v>
+        <v>0.0062588</v>
       </c>
       <c r="F41" t="n">
-        <v>0.023157</v>
+        <v>0.023156</v>
       </c>
     </row>
     <row r="42">
@@ -1359,16 +1359,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.0005820000000000001</v>
+        <v>0.0007851000000000001</v>
       </c>
       <c r="D42" t="n">
-        <v>0.001799</v>
+        <v>0.001794</v>
       </c>
       <c r="E42" t="n">
-        <v>0.005866</v>
+        <v>0.0057219</v>
       </c>
       <c r="F42" t="n">
-        <v>0.021985</v>
+        <v>0.0216487</v>
       </c>
     </row>
     <row r="43">
@@ -1381,16 +1381,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.000599</v>
+        <v>0.0005863</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0023</v>
+        <v>0.0022057</v>
       </c>
       <c r="E43" t="n">
-        <v>0.008387</v>
+        <v>0.0083985</v>
       </c>
       <c r="F43" t="n">
-        <v>0.031853</v>
+        <v>0.0317342</v>
       </c>
     </row>
     <row r="44">
@@ -1403,16 +1403,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.000635</v>
+        <v>0.0006259</v>
       </c>
       <c r="D44" t="n">
-        <v>0.002589</v>
+        <v>0.0025473</v>
       </c>
       <c r="E44" t="n">
-        <v>0.012559</v>
+        <v>0.0121728</v>
       </c>
       <c r="F44" t="n">
-        <v>0.057593</v>
+        <v>0.05622820000000001</v>
       </c>
     </row>
     <row r="45">
@@ -1425,16 +1425,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.000602</v>
+        <v>0.0006152</v>
       </c>
       <c r="D45" t="n">
-        <v>0.002822</v>
+        <v>0.0027448</v>
       </c>
       <c r="E45" t="n">
-        <v>0.012489</v>
+        <v>0.0121276</v>
       </c>
       <c r="F45" t="n">
-        <v>0.061989</v>
+        <v>0.0602138</v>
       </c>
     </row>
     <row r="46">
@@ -1447,16 +1447,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.000589</v>
+        <v>0.0005870000000000001</v>
       </c>
       <c r="D46" t="n">
-        <v>0.002877</v>
+        <v>0.0026965</v>
       </c>
       <c r="E46" t="n">
-        <v>0.011916</v>
+        <v>0.0124019</v>
       </c>
       <c r="F46" t="n">
-        <v>0.057719</v>
+        <v>0.05677260000000001</v>
       </c>
     </row>
     <row r="47">
@@ -1469,16 +1469,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.000504</v>
+        <v>0.000463</v>
       </c>
       <c r="D47" t="n">
-        <v>0.001864</v>
+        <v>0.0018411</v>
       </c>
       <c r="E47" t="n">
-        <v>0.007581</v>
+        <v>0.0075125</v>
       </c>
       <c r="F47" t="n">
-        <v>0.033276</v>
+        <v>0.0329598</v>
       </c>
     </row>
     <row r="48">
@@ -1491,16 +1491,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.001082</v>
+        <v>0.0010996</v>
       </c>
       <c r="D48" t="n">
-        <v>0.006039</v>
+        <v>0.0060618</v>
       </c>
       <c r="E48" t="n">
-        <v>0.034748</v>
+        <v>0.034476</v>
       </c>
       <c r="F48" t="n">
-        <v>0.229446</v>
+        <v>0.2246846</v>
       </c>
     </row>
     <row r="49">
@@ -1513,16 +1513,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.000486</v>
+        <v>0.0004598</v>
       </c>
       <c r="D49" t="n">
-        <v>0.001322</v>
+        <v>0.0013575</v>
       </c>
       <c r="E49" t="n">
-        <v>0.004307</v>
+        <v>0.0040994</v>
       </c>
       <c r="F49" t="n">
-        <v>0.014104</v>
+        <v>0.0140587</v>
       </c>
     </row>
     <row r="50">
@@ -1535,16 +1535,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.000449</v>
+        <v>0.0004359</v>
       </c>
       <c r="D50" t="n">
-        <v>0.001304</v>
+        <v>0.0012977</v>
       </c>
       <c r="E50" t="n">
-        <v>0.004058</v>
+        <v>0.0039259</v>
       </c>
       <c r="F50" t="n">
-        <v>0.015346</v>
+        <v>0.0153188</v>
       </c>
     </row>
     <row r="51">
@@ -1557,16 +1557,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.000356</v>
+        <v>0.0003382</v>
       </c>
       <c r="D51" t="n">
-        <v>0.000937</v>
+        <v>0.0009304</v>
       </c>
       <c r="E51" t="n">
-        <v>0.003053</v>
+        <v>0.0029938</v>
       </c>
       <c r="F51" t="n">
-        <v>0.011238</v>
+        <v>0.0110146</v>
       </c>
     </row>
     <row r="52">
@@ -1579,16 +1579,16 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.000339</v>
+        <v>0.000315</v>
       </c>
       <c r="D52" t="n">
-        <v>0.000973</v>
+        <v>0.0009437000000000001</v>
       </c>
       <c r="E52" t="n">
-        <v>0.003218</v>
+        <v>0.0029947</v>
       </c>
       <c r="F52" t="n">
-        <v>0.010886</v>
+        <v>0.0110853</v>
       </c>
     </row>
     <row r="53">
@@ -1601,16 +1601,16 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.000313</v>
+        <v>0.0002847</v>
       </c>
       <c r="D53" t="n">
-        <v>0.000951</v>
+        <v>0.0009411000000000001</v>
       </c>
       <c r="E53" t="n">
-        <v>0.003884</v>
+        <v>0.0038757</v>
       </c>
       <c r="F53" t="n">
-        <v>0.019544</v>
+        <v>0.0189742</v>
       </c>
     </row>
     <row r="54">
@@ -1623,16 +1623,16 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.000446</v>
+        <v>0.0004332</v>
       </c>
       <c r="D54" t="n">
-        <v>0.001251</v>
+        <v>0.0012368</v>
       </c>
       <c r="E54" t="n">
-        <v>0.004201</v>
+        <v>0.0042067</v>
       </c>
       <c r="F54" t="n">
-        <v>0.018897</v>
+        <v>0.019395</v>
       </c>
     </row>
     <row r="55">
@@ -1645,16 +1645,16 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.000552</v>
+        <v>0.0005053</v>
       </c>
       <c r="D55" t="n">
-        <v>0.001572</v>
+        <v>0.0018536</v>
       </c>
       <c r="E55" t="n">
-        <v>0.003922</v>
+        <v>0.0039446</v>
       </c>
       <c r="F55" t="n">
-        <v>0.013043</v>
+        <v>0.0132029</v>
       </c>
     </row>
     <row r="56">
@@ -1667,16 +1667,16 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.000566</v>
+        <v>0.0005484</v>
       </c>
       <c r="D56" t="n">
-        <v>0.001627</v>
+        <v>0.0018039</v>
       </c>
       <c r="E56" t="n">
-        <v>0.005027</v>
+        <v>0.0046199</v>
       </c>
       <c r="F56" t="n">
-        <v>0.017002</v>
+        <v>0.0169609</v>
       </c>
     </row>
     <row r="57">
@@ -1689,16 +1689,16 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.0005330000000000001</v>
+        <v>0.0005174999999999999</v>
       </c>
       <c r="D57" t="n">
-        <v>0.001705</v>
+        <v>0.0015884</v>
       </c>
       <c r="E57" t="n">
-        <v>0.004712</v>
+        <v>0.0045138</v>
       </c>
       <c r="F57" t="n">
-        <v>0.016765</v>
+        <v>0.0167245</v>
       </c>
     </row>
     <row r="58">
@@ -1711,16 +1711,16 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.000618</v>
+        <v>0.0008805999999999999</v>
       </c>
       <c r="D58" t="n">
-        <v>0.001909</v>
+        <v>0.0019634</v>
       </c>
       <c r="E58" t="n">
-        <v>0.005931</v>
+        <v>0.00589</v>
       </c>
       <c r="F58" t="n">
-        <v>0.02168</v>
+        <v>0.0218002</v>
       </c>
     </row>
     <row r="59">
@@ -1733,16 +1733,16 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.0006310000000000001</v>
+        <v>0.0006466</v>
       </c>
       <c r="D59" t="n">
-        <v>0.002818</v>
+        <v>0.002751</v>
       </c>
       <c r="E59" t="n">
-        <v>0.012976</v>
+        <v>0.0117828</v>
       </c>
       <c r="F59" t="n">
-        <v>0.059253</v>
+        <v>0.0577711</v>
       </c>
     </row>
     <row r="60">
@@ -1755,16 +1755,16 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.000491</v>
+        <v>0.0004894000000000001</v>
       </c>
       <c r="D60" t="n">
-        <v>0.001415</v>
+        <v>0.0013653</v>
       </c>
       <c r="E60" t="n">
-        <v>0.00412</v>
+        <v>0.0039968</v>
       </c>
       <c r="F60" t="n">
-        <v>0.015545</v>
+        <v>0.0156394</v>
       </c>
     </row>
     <row r="61">
@@ -1777,16 +1777,16 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.000382</v>
+        <v>0.0003649</v>
       </c>
       <c r="D61" t="n">
-        <v>0.001007</v>
+        <v>0.0010021</v>
       </c>
       <c r="E61" t="n">
-        <v>0.003074</v>
+        <v>0.0031207</v>
       </c>
       <c r="F61" t="n">
-        <v>0.01122</v>
+        <v>0.0111789</v>
       </c>
     </row>
     <row r="62">
@@ -1799,16 +1799,16 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.000344</v>
+        <v>0.0003525000000000001</v>
       </c>
       <c r="D62" t="n">
-        <v>0.0009990000000000001</v>
+        <v>0.0010047</v>
       </c>
       <c r="E62" t="n">
-        <v>0.003532</v>
+        <v>0.0034927</v>
       </c>
       <c r="F62" t="n">
-        <v>0.017579</v>
+        <v>0.0175678</v>
       </c>
     </row>
     <row r="63">
@@ -1821,16 +1821,16 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.000348</v>
+        <v>0.0003398</v>
       </c>
       <c r="D63" t="n">
-        <v>0.001031</v>
+        <v>0.0010053</v>
       </c>
       <c r="E63" t="n">
-        <v>0.004005</v>
+        <v>0.0039298</v>
       </c>
       <c r="F63" t="n">
-        <v>0.019042</v>
+        <v>0.0191615</v>
       </c>
     </row>
     <row r="64">
@@ -1843,16 +1843,16 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.000584</v>
+        <v>0.0005579</v>
       </c>
       <c r="D64" t="n">
-        <v>0.001773</v>
+        <v>0.0016534</v>
       </c>
       <c r="E64" t="n">
-        <v>0.004722</v>
+        <v>0.0046043</v>
       </c>
       <c r="F64" t="n">
-        <v>0.017121</v>
+        <v>0.017154</v>
       </c>
     </row>
     <row r="65">
@@ -1865,16 +1865,16 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.000387</v>
+        <v>0.0003860000000000001</v>
       </c>
       <c r="D65" t="n">
-        <v>0.001059</v>
+        <v>0.0010659</v>
       </c>
       <c r="E65" t="n">
-        <v>0.003702</v>
+        <v>0.003652</v>
       </c>
       <c r="F65" t="n">
-        <v>0.018284</v>
+        <v>0.0180251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>